<commit_message>
BraunUS updated code helper, TestExecute, resources.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/BraunHC/BraunHCTestData.xlsx
+++ b/src/test/resources/TestData/BraunHC/BraunHCTestData.xlsx
@@ -5,27 +5,36 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\HoT-digital\HoT-digital\src\test\resources\TestData\BraunHC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NEW_code\HoT-digital\src\test\resources\TestData\BraunHC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE5F9E1-6E38-4486-98EF-9E3AD012732D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9981676E-90B1-403B-82AB-423AD459408F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B7D300D1-7AEC-4306-B2B0-C9F210226332}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="133">
   <si>
     <t>DataSet</t>
   </si>
@@ -400,6 +409,30 @@
   </si>
   <si>
     <t>braunhealthcare@gmail.com</t>
+  </si>
+  <si>
+    <t>NoTaxShippingAddress</t>
+  </si>
+  <si>
+    <t>4 Highland Ter</t>
+  </si>
+  <si>
+    <t>South Burlington</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>Braunus123@gmail.com</t>
+  </si>
+  <si>
+    <t>Wallingford</t>
+  </si>
+  <si>
+    <t>06492</t>
+  </si>
+  <si>
+    <t>CustomerAccountdetails</t>
   </si>
 </sst>
 </file>
@@ -409,7 +442,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,6 +477,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -500,7 +539,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -523,6 +562,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -838,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5AA4073-2E49-4649-9D78-B3EDA801FEDE}">
-  <dimension ref="A1:AM29"/>
+  <dimension ref="A1:AM31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD15" workbookViewId="0">
-      <selection activeCell="AK24" sqref="AK24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +897,7 @@
     <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
@@ -988,9 +1030,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>30</v>
+    <row r="2" spans="1:39" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>132</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>124</v>
@@ -998,10 +1040,10 @@
       <c r="C2" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="12" t="s">
         <v>93</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1010,10 +1052,10 @@
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>121</v>
@@ -1024,73 +1066,77 @@
       <c r="E3" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="D4" t="s">
         <v>123</v>
       </c>
       <c r="E4" t="s">
         <v>93</v>
       </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4">
-        <v>12345</v>
-      </c>
-      <c r="M4" s="3">
-        <v>9898989899</v>
-      </c>
-      <c r="N4" s="3"/>
+      <c r="F4" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="O5" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>2021</v>
-      </c>
-      <c r="R5" t="s">
-        <v>41</v>
-      </c>
-      <c r="S5" s="3">
-        <v>737</v>
-      </c>
+      <c r="D5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>130</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="M5" s="3">
+        <v>9898989899</v>
+      </c>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2"/>
       <c r="O6" t="s">
         <v>39</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="Q6" s="5">
         <v>2021</v>
@@ -1104,84 +1150,48 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="T7" t="s">
-        <v>45</v>
-      </c>
-      <c r="U7" t="s">
-        <v>46</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>48</v>
+      <c r="O7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>2021</v>
+      </c>
+      <c r="R7" t="s">
+        <v>41</v>
+      </c>
+      <c r="S7" s="3">
+        <v>737</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J8" t="s">
-        <v>74</v>
-      </c>
-      <c r="K8" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8">
-        <v>12345</v>
-      </c>
-      <c r="M8" s="3">
-        <v>9898989899</v>
-      </c>
-      <c r="N8" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
       <c r="T8" t="s">
         <v>45</v>
       </c>
       <c r="U8" t="s">
-        <v>51</v>
-      </c>
-      <c r="X8">
-        <v>12341</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z8">
-        <v>5</v>
-      </c>
-      <c r="AA8">
-        <v>6</v>
-      </c>
-      <c r="AB8">
-        <v>2020</v>
+        <v>46</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
         <v>123</v>
@@ -1202,7 +1212,7 @@
         <v>49</v>
       </c>
       <c r="J9" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="K9" t="s">
         <v>50</v>
@@ -1238,7 +1248,7 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
         <v>123</v>
@@ -1250,199 +1260,240 @@
         <v>122</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="H10" t="s">
         <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="J10" t="s">
-        <v>107</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>108</v>
-      </c>
-      <c r="L10" s="6">
-        <v>98569</v>
+        <v>50</v>
+      </c>
+      <c r="L10">
+        <v>12345</v>
       </c>
       <c r="M10" s="3">
         <v>9898989899</v>
       </c>
-      <c r="N10" s="9" t="s">
-        <v>110</v>
+      <c r="N10" s="3"/>
+      <c r="T10" t="s">
+        <v>45</v>
+      </c>
+      <c r="U10" t="s">
+        <v>51</v>
+      </c>
+      <c r="X10">
+        <v>12341</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z10">
+        <v>5</v>
+      </c>
+      <c r="AA10">
+        <v>6</v>
+      </c>
+      <c r="AB10">
+        <v>2020</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="T11" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" t="s">
+        <v>107</v>
+      </c>
+      <c r="K11" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" s="6">
+        <v>98569</v>
+      </c>
+      <c r="M11" s="3">
+        <v>9898989899</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" t="s">
-        <v>123</v>
-      </c>
-      <c r="E12" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" t="s">
-        <v>55</v>
+        <v>18</v>
+      </c>
+      <c r="T12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
-      </c>
-      <c r="T13" s="6" t="s">
-        <v>106</v>
+        <v>58</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>86</v>
+      </c>
+      <c r="J14">
+        <f>+K12</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
-      </c>
-      <c r="T15" s="6" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" t="s">
-        <v>123</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="T17" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>70</v>
       </c>
-      <c r="AE19" t="s">
+      <c r="AE20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="T20" t="s">
+      <c r="T21" t="s">
         <v>72</v>
       </c>
-      <c r="AF20" t="s">
+      <c r="AF21" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" t="s">
-        <v>123</v>
-      </c>
-      <c r="E21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G21" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" t="s">
-        <v>49</v>
-      </c>
-      <c r="J21" t="s">
-        <v>74</v>
-      </c>
-      <c r="K21" t="s">
-        <v>56</v>
-      </c>
-      <c r="L21">
-        <v>12345</v>
-      </c>
-      <c r="M21" s="3">
-        <v>9898989899</v>
-      </c>
-      <c r="N21" s="3"/>
-      <c r="AG21">
-        <v>8444</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>76</v>
-      </c>
-      <c r="O22" t="s">
-        <v>77</v>
-      </c>
-      <c r="P22" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q22">
-        <v>2023</v>
-      </c>
-      <c r="R22" t="s">
-        <v>41</v>
-      </c>
-      <c r="S22">
-        <v>731</v>
+        <v>75</v>
+      </c>
+      <c r="D22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" t="s">
+        <v>74</v>
+      </c>
+      <c r="K22" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22">
+        <v>12345</v>
+      </c>
+      <c r="M22" s="3">
+        <v>9898989899</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="AG22">
+        <v>8444</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="O23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="Q23">
         <v>2023</v>
@@ -1456,13 +1507,13 @@
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="O24" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q24">
         <v>2023</v>
@@ -1471,53 +1522,38 @@
         <v>41</v>
       </c>
       <c r="S24">
-        <v>314</v>
-      </c>
-      <c r="AH24">
-        <v>25376</v>
-      </c>
-      <c r="AI24" t="s">
-        <v>105</v>
+        <v>731</v>
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D25" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G25" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" t="s">
-        <v>93</v>
-      </c>
-      <c r="J25" t="s">
-        <v>94</v>
-      </c>
-      <c r="K25" t="s">
-        <v>37</v>
-      </c>
-      <c r="L25">
-        <v>23456</v>
-      </c>
-      <c r="M25">
-        <v>8897006543</v>
-      </c>
-      <c r="T25" t="s">
-        <v>106</v>
+        <v>79</v>
+      </c>
+      <c r="O25" t="s">
+        <v>80</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q25">
+        <v>2023</v>
+      </c>
+      <c r="R25" t="s">
+        <v>41</v>
+      </c>
+      <c r="S25">
+        <v>9876</v>
+      </c>
+      <c r="AH25">
+        <v>25376</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
         <v>123</v>
@@ -1526,119 +1562,196 @@
         <v>93</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="G26" t="s">
-        <v>95</v>
-      </c>
-      <c r="H26" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I26" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J26" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="K26" t="s">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="L26">
-        <v>98987</v>
+        <v>23456</v>
       </c>
       <c r="M26">
-        <v>9898908878</v>
+        <v>8897006543</v>
       </c>
       <c r="T26" t="s">
-        <v>100</v>
-      </c>
-      <c r="AK26">
-        <v>3400000747</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM27">
-        <v>2</v>
+        <v>91</v>
+      </c>
+      <c r="D27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J27" t="s">
+        <v>98</v>
+      </c>
+      <c r="K27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L27">
+        <v>98987</v>
+      </c>
+      <c r="M27">
+        <v>9898908878</v>
+      </c>
+      <c r="T27" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK27">
+        <v>3400000747</v>
       </c>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E28" t="s">
-        <v>115</v>
-      </c>
-      <c r="G28" t="s">
-        <v>33</v>
-      </c>
-      <c r="H28" t="s">
-        <v>96</v>
-      </c>
-      <c r="I28" t="s">
-        <v>49</v>
-      </c>
-      <c r="J28" t="s">
-        <v>74</v>
-      </c>
-      <c r="K28" t="s">
-        <v>108</v>
-      </c>
-      <c r="L28">
-        <v>71823</v>
-      </c>
-      <c r="M28">
-        <v>9898989898</v>
+        <v>111</v>
+      </c>
+      <c r="AM28">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D29" t="s">
         <v>114</v>
       </c>
       <c r="E29" t="s">
+        <v>115</v>
+      </c>
+      <c r="G29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" t="s">
+        <v>49</v>
+      </c>
+      <c r="J29" t="s">
+        <v>74</v>
+      </c>
+      <c r="K29" t="s">
+        <v>108</v>
+      </c>
+      <c r="L29">
+        <v>71823</v>
+      </c>
+      <c r="M29">
+        <v>9898989898</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" t="s">
         <v>117</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G30" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H30" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="I29" s="10" t="s">
+      <c r="I30" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J29" s="13" t="s">
+      <c r="J30" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="K29" s="12" t="s">
+      <c r="K30" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="L29" s="12">
+      <c r="L30" s="12">
         <v>98987</v>
       </c>
-      <c r="M29" s="12">
+      <c r="M30" s="12">
+        <v>8897006543</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J31" t="s">
+        <v>127</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="L31" s="15">
+        <v>5403</v>
+      </c>
+      <c r="M31" s="12">
         <v>8897006543</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="V7" r:id="rId1" xr:uid="{FD2FF487-3C23-4A89-AB86-AB47176DE319}"/>
-    <hyperlink ref="W7" r:id="rId2" xr:uid="{6A81ABFC-B64F-4571-86FD-66321CB54E70}"/>
-    <hyperlink ref="F8" r:id="rId3" xr:uid="{7B998F73-6B03-4231-B2E7-D1AF98C503AD}"/>
-    <hyperlink ref="B12" r:id="rId4" xr:uid="{B34FA12C-9F7E-4F04-BB36-292100CCE8A7}"/>
-    <hyperlink ref="F9:F10" r:id="rId5" display="BraunUs@gmail.com" xr:uid="{55CEB419-6BF0-4280-AE74-E8F9C00802FB}"/>
-    <hyperlink ref="F26" r:id="rId6" xr:uid="{C027A678-1C8F-44F8-B9BA-5F614384249A}"/>
+    <hyperlink ref="V8" r:id="rId1" xr:uid="{FD2FF487-3C23-4A89-AB86-AB47176DE319}"/>
+    <hyperlink ref="W8" r:id="rId2" xr:uid="{6A81ABFC-B64F-4571-86FD-66321CB54E70}"/>
+    <hyperlink ref="F9" r:id="rId3" xr:uid="{7B998F73-6B03-4231-B2E7-D1AF98C503AD}"/>
+    <hyperlink ref="B13" r:id="rId4" xr:uid="{B34FA12C-9F7E-4F04-BB36-292100CCE8A7}"/>
+    <hyperlink ref="F10:F11" r:id="rId5" display="BraunUs@gmail.com" xr:uid="{55CEB419-6BF0-4280-AE74-E8F9C00802FB}"/>
+    <hyperlink ref="F18" r:id="rId6" xr:uid="{20C69D56-8C61-4EB3-B742-4C91A5353615}"/>
+    <hyperlink ref="F22" r:id="rId7" xr:uid="{E76C52E7-8539-4503-8F36-04FEAA7C6F4B}"/>
+    <hyperlink ref="F26" r:id="rId8" xr:uid="{345711FA-1E5F-4C3C-8FF4-29295C109D17}"/>
+    <hyperlink ref="F27" r:id="rId9" xr:uid="{665EF1F8-980B-43D0-9E53-AE3F7CB643D6}"/>
+    <hyperlink ref="F31" r:id="rId10" xr:uid="{5F948262-4CF2-42FF-8B86-A6065F1BA003}"/>
+    <hyperlink ref="F5" r:id="rId11" xr:uid="{87DDA46A-A20A-4643-BB81-1C7CF7F6C798}"/>
+    <hyperlink ref="F4" r:id="rId12" xr:uid="{DF65CA92-314B-400B-8AE1-F2324391B535}"/>
+    <hyperlink ref="C2" r:id="rId13" xr:uid="{474DDF44-173E-49F7-BF59-B58BB733B18D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove BraunUS test execute old code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/BraunHC/BraunHCTestData.xlsx
+++ b/src/test/resources/TestData/BraunHC/BraunHCTestData.xlsx
@@ -1,40 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NEW_code\HoT-digital\src\test\resources\TestData\BraunHC\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9981676E-90B1-403B-82AB-423AD459408F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DF929C3D-59D8-4E37-A6AA-5B079C7423B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B7D300D1-7AEC-4306-B2B0-C9F210226332}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20760" windowHeight="11820" xr2:uid="{B7D300D1-7AEC-4306-B2B0-C9F210226332}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="134">
   <si>
     <t>DataSet</t>
   </si>
@@ -433,6 +420,9 @@
   </si>
   <si>
     <t>CustomerAccountdetails</t>
+  </si>
+  <si>
+    <t>..</t>
   </si>
 </sst>
 </file>
@@ -880,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5AA4073-2E49-4649-9D78-B3EDA801FEDE}">
-  <dimension ref="A1:AM31"/>
+  <dimension ref="A1:AM32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,6 +1084,7 @@
       <c r="A5" t="s">
         <v>32</v>
       </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
         <v>123</v>
@@ -1732,6 +1723,11 @@
       </c>
       <c r="M31" s="12">
         <v>8897006543</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Braun US Updated code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/BraunHC/BraunHCTestData.xlsx
+++ b/src/test/resources/TestData/BraunHC/BraunHCTestData.xlsx
@@ -1,34 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DF929C3D-59D8-4E37-A6AA-5B079C7423B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stage1\HoT-digital\src\test\resources\TestData\BraunHC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3AF648-6555-4F43-B9C8-696101DEFB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20760" windowHeight="11820" xr2:uid="{B7D300D1-7AEC-4306-B2B0-C9F210226332}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="139">
   <si>
     <t>DataSet</t>
   </si>
   <si>
-    <t>UserName</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -131,9 +141,6 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Concord</t>
-  </si>
-  <si>
     <t>California</t>
   </si>
   <si>
@@ -182,9 +189,6 @@
     <t>Nice Product</t>
   </si>
   <si>
-    <t>Product_Registration</t>
-  </si>
-  <si>
     <t>Guest_shipping</t>
   </si>
   <si>
@@ -377,12 +381,6 @@
     <t>Bethi</t>
   </si>
   <si>
-    <t>Peach Orchard</t>
-  </si>
-  <si>
-    <t>13 Annadale Ave. Peach Orchard</t>
-  </si>
-  <si>
     <t xml:space="preserve"> dtc.qatesting.braunus@gmail.com</t>
   </si>
   <si>
@@ -395,9 +393,6 @@
     <t>Braun</t>
   </si>
   <si>
-    <t>braunhealthcare@gmail.com</t>
-  </si>
-  <si>
     <t>NoTaxShippingAddress</t>
   </si>
   <si>
@@ -422,7 +417,41 @@
     <t>CustomerAccountdetails</t>
   </si>
   <si>
-    <t>..</t>
+    <t>Very good product</t>
+  </si>
+  <si>
+    <t>05403</t>
+  </si>
+  <si>
+    <t>3224 Sandy Ln</t>
+  </si>
+  <si>
+    <t>Glenview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approximate Date of Purchase </t>
+  </si>
+  <si>
+    <t>Thursday, October 21, 2021</t>
+  </si>
+  <si>
+    <t>BraunUs</t>
+  </si>
+  <si>
+    <t>healthcare</t>
+  </si>
+  <si>
+    <t>divya@123456</t>
+  </si>
+  <si>
+    <t>Braunusqatester@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Braunusqatester@gmail.com</t>
+  </si>
+  <si>
+    <t>Guam</t>
   </si>
 </sst>
 </file>
@@ -432,7 +461,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,6 +502,13 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -529,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -553,8 +589,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -869,11 +908,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5AA4073-2E49-4649-9D78-B3EDA801FEDE}">
-  <dimension ref="A1:AM32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AN30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,319 +933,327 @@
     <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.140625" customWidth="1"/>
+    <col min="24" max="24" width="14.140625" customWidth="1"/>
+    <col min="25" max="25" width="17.42578125" customWidth="1"/>
     <col min="31" max="31" width="72.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="22" customWidth="1"/>
     <col min="33" max="33" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.42578125" customWidth="1"/>
+    <col min="35" max="35" width="29.42578125" customWidth="1"/>
     <col min="36" max="36" width="16.5703125" customWidth="1"/>
     <col min="37" max="37" width="22.5703125" customWidth="1"/>
+    <col min="40" max="40" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:40" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
         <v>34</v>
       </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
       <c r="J5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>131</v>
+        <v>53</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>125</v>
       </c>
       <c r="M5" s="3">
         <v>9898989899</v>
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2"/>
       <c r="O6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>2030</v>
+      </c>
+      <c r="R6" t="s">
         <v>39</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>2021</v>
-      </c>
-      <c r="R6" t="s">
-        <v>41</v>
       </c>
       <c r="S6" s="3">
         <v>737</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2"/>
       <c r="O7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>2030</v>
+      </c>
+      <c r="R7" t="s">
         <v>39</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>2021</v>
-      </c>
-      <c r="R7" t="s">
-        <v>41</v>
       </c>
       <c r="S7" s="3">
         <v>737</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="T8" t="s">
+        <v>43</v>
+      </c>
+      <c r="U8" t="s">
+        <v>44</v>
+      </c>
+      <c r="V8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="U8" t="s">
+      <c r="W8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="V8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" t="s">
         <v>47</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="J9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" t="s">
-        <v>74</v>
-      </c>
-      <c r="K9" t="s">
-        <v>50</v>
       </c>
       <c r="L9">
         <v>12345</v>
@@ -1216,16 +1263,16 @@
       </c>
       <c r="N9" s="3"/>
       <c r="T9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="U9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="X9">
         <v>12341</v>
       </c>
       <c r="Y9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Z9">
         <v>5</v>
@@ -1237,159 +1284,119 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" t="s">
         <v>33</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>34</v>
       </c>
-      <c r="I10" t="s">
-        <v>49</v>
-      </c>
       <c r="J10" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="K10" t="s">
-        <v>50</v>
-      </c>
-      <c r="L10">
-        <v>12345</v>
+        <v>105</v>
+      </c>
+      <c r="L10" s="6">
+        <v>98569</v>
       </c>
       <c r="M10" s="3">
         <v>9898989899</v>
       </c>
-      <c r="N10" s="3"/>
-      <c r="T10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U10" t="s">
-        <v>51</v>
-      </c>
-      <c r="X10">
-        <v>12341</v>
-      </c>
-      <c r="Y10" t="s">
+      <c r="N10" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="T11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" t="s">
         <v>52</v>
       </c>
-      <c r="Z10">
-        <v>5</v>
-      </c>
-      <c r="AA10">
-        <v>6</v>
-      </c>
-      <c r="AB10">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" t="s">
-        <v>123</v>
-      </c>
-      <c r="E11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G11" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" t="s">
-        <v>107</v>
-      </c>
-      <c r="K11" t="s">
-        <v>108</v>
-      </c>
-      <c r="L11" s="6">
-        <v>98569</v>
-      </c>
-      <c r="M11" s="3">
-        <v>9898989899</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="T12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13">
+        <f>+K11</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="2" t="s">
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>59</v>
       </c>
-      <c r="C13" t="s">
+      <c r="T15" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>60</v>
       </c>
-      <c r="D13" t="s">
-        <v>123</v>
-      </c>
-      <c r="E13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>86</v>
-      </c>
-      <c r="J14">
-        <f>+K12</f>
-        <v>0</v>
-      </c>
-      <c r="T14" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="T16" s="6" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>62</v>
-      </c>
-      <c r="T16" s="6" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC17" t="s">
         <v>63</v>
       </c>
-      <c r="T17" s="6" t="s">
+      <c r="AD17" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1397,100 +1404,103 @@
       <c r="A18" t="s">
         <v>65</v>
       </c>
-      <c r="D18" t="s">
-        <v>123</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="AC18" t="s">
+      <c r="AE18" t="s">
         <v>66</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE19" t="s">
         <v>68</v>
       </c>
-      <c r="AE19" t="s">
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="T20" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE20" t="s">
+      <c r="AF20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" t="s">
+        <v>47</v>
+      </c>
+      <c r="J21" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="T21" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF21" t="s">
-        <v>88</v>
+      <c r="K21" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21">
+        <v>12345</v>
+      </c>
+      <c r="M21" s="3">
+        <v>9898989899</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="AG21">
+        <v>8444</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" t="s">
-        <v>123</v>
-      </c>
-      <c r="E22" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" t="s">
-        <v>34</v>
-      </c>
-      <c r="I22" t="s">
-        <v>49</v>
-      </c>
-      <c r="J22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O22" t="s">
         <v>74</v>
       </c>
-      <c r="K22" t="s">
-        <v>56</v>
-      </c>
-      <c r="L22">
-        <v>12345</v>
-      </c>
-      <c r="M22" s="3">
-        <v>9898989899</v>
-      </c>
-      <c r="N22" s="3"/>
-      <c r="AG22">
-        <v>8444</v>
+      <c r="P22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q22">
+        <v>2030</v>
+      </c>
+      <c r="R22" t="s">
+        <v>39</v>
+      </c>
+      <c r="S22">
+        <v>731</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="O23" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="Q23">
-        <v>2023</v>
+        <v>2030</v>
       </c>
       <c r="R23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="S23">
         <v>731</v>
@@ -1498,132 +1508,159 @@
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="O24" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="P24" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="Q24">
-        <v>2023</v>
+      <c r="Q24" s="12">
+        <v>2030</v>
       </c>
       <c r="R24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="S24">
-        <v>731</v>
+        <v>9876</v>
+      </c>
+      <c r="AH24">
+        <v>25376</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>79</v>
-      </c>
-      <c r="O25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P25" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q25">
-        <v>2023</v>
-      </c>
-      <c r="R25" t="s">
-        <v>41</v>
-      </c>
-      <c r="S25">
-        <v>9876</v>
+        <v>87</v>
+      </c>
+      <c r="D25" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K25" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25">
+        <v>23456</v>
+      </c>
+      <c r="M25">
+        <v>8897006543</v>
+      </c>
+      <c r="T25" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y25" s="12" t="s">
+        <v>127</v>
       </c>
       <c r="AH25">
-        <v>25376</v>
+        <v>9876543210</v>
       </c>
       <c r="AI25" t="s">
-        <v>105</v>
+        <v>132</v>
+      </c>
+      <c r="AJ25">
+        <v>56789</v>
       </c>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D26" t="s">
+        <v>133</v>
+      </c>
+      <c r="E26" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="E26" t="s">
-        <v>93</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="G26" t="s">
         <v>92</v>
       </c>
+      <c r="H26" t="s">
+        <v>93</v>
+      </c>
       <c r="I26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K26" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="L26">
-        <v>23456</v>
+        <v>98987</v>
       </c>
       <c r="M26">
-        <v>8897006543</v>
+        <v>9898908878</v>
       </c>
       <c r="T26" t="s">
-        <v>106</v>
+        <v>97</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK26">
+        <v>3400000747</v>
       </c>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" t="s">
-        <v>123</v>
-      </c>
-      <c r="E27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G27" t="s">
-        <v>95</v>
-      </c>
-      <c r="H27" t="s">
-        <v>96</v>
-      </c>
-      <c r="I27" t="s">
-        <v>97</v>
-      </c>
-      <c r="J27" t="s">
-        <v>98</v>
-      </c>
-      <c r="K27" t="s">
-        <v>99</v>
-      </c>
-      <c r="L27">
-        <v>98987</v>
-      </c>
-      <c r="M27">
-        <v>9898908878</v>
-      </c>
-      <c r="T27" t="s">
-        <v>100</v>
-      </c>
-      <c r="AK27">
-        <v>3400000747</v>
+        <v>108</v>
+      </c>
+      <c r="AM27">
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" t="s">
         <v>111</v>
       </c>
-      <c r="AM28">
-        <v>2</v>
+      <c r="E28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" t="s">
+        <v>93</v>
+      </c>
+      <c r="I28" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" t="s">
+        <v>71</v>
+      </c>
+      <c r="K28" t="s">
+        <v>105</v>
+      </c>
+      <c r="L28">
+        <v>71823</v>
+      </c>
+      <c r="M28">
+        <v>9898989898</v>
       </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
@@ -1631,123 +1668,85 @@
         <v>113</v>
       </c>
       <c r="D29" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" t="s">
         <v>114</v>
       </c>
-      <c r="E29" t="s">
-        <v>115</v>
-      </c>
-      <c r="G29" t="s">
-        <v>33</v>
-      </c>
-      <c r="H29" t="s">
-        <v>96</v>
-      </c>
-      <c r="I29" t="s">
-        <v>49</v>
-      </c>
-      <c r="J29" t="s">
-        <v>74</v>
-      </c>
-      <c r="K29" t="s">
-        <v>108</v>
-      </c>
-      <c r="L29">
-        <v>71823</v>
-      </c>
-      <c r="M29">
-        <v>9898989898</v>
+      <c r="G29" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L29" s="12">
+        <v>60026</v>
+      </c>
+      <c r="M29" s="12">
+        <v>8897006543</v>
       </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>116</v>
-      </c>
-      <c r="D30" t="s">
-        <v>114</v>
-      </c>
-      <c r="E30" t="s">
-        <v>117</v>
-      </c>
-      <c r="G30" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H30" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="J30" s="13" t="s">
+      <c r="D30" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="K30" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L30" s="12">
-        <v>98987</v>
+      <c r="E30" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J30" t="s">
+        <v>121</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="L30" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="M30" s="12">
         <v>8897006543</v>
-      </c>
-    </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>125</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J31" t="s">
-        <v>127</v>
-      </c>
-      <c r="K31" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="L31" s="15">
-        <v>5403</v>
-      </c>
-      <c r="M31" s="12">
-        <v>8897006543</v>
-      </c>
-    </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="V8" r:id="rId1" xr:uid="{FD2FF487-3C23-4A89-AB86-AB47176DE319}"/>
-    <hyperlink ref="W8" r:id="rId2" xr:uid="{6A81ABFC-B64F-4571-86FD-66321CB54E70}"/>
-    <hyperlink ref="F9" r:id="rId3" xr:uid="{7B998F73-6B03-4231-B2E7-D1AF98C503AD}"/>
-    <hyperlink ref="B13" r:id="rId4" xr:uid="{B34FA12C-9F7E-4F04-BB36-292100CCE8A7}"/>
-    <hyperlink ref="F10:F11" r:id="rId5" display="BraunUs@gmail.com" xr:uid="{55CEB419-6BF0-4280-AE74-E8F9C00802FB}"/>
-    <hyperlink ref="F18" r:id="rId6" xr:uid="{20C69D56-8C61-4EB3-B742-4C91A5353615}"/>
-    <hyperlink ref="F22" r:id="rId7" xr:uid="{E76C52E7-8539-4503-8F36-04FEAA7C6F4B}"/>
-    <hyperlink ref="F26" r:id="rId8" xr:uid="{345711FA-1E5F-4C3C-8FF4-29295C109D17}"/>
-    <hyperlink ref="F27" r:id="rId9" xr:uid="{665EF1F8-980B-43D0-9E53-AE3F7CB643D6}"/>
-    <hyperlink ref="F31" r:id="rId10" xr:uid="{5F948262-4CF2-42FF-8B86-A6065F1BA003}"/>
-    <hyperlink ref="F5" r:id="rId11" xr:uid="{87DDA46A-A20A-4643-BB81-1C7CF7F6C798}"/>
-    <hyperlink ref="F4" r:id="rId12" xr:uid="{DF65CA92-314B-400B-8AE1-F2324391B535}"/>
-    <hyperlink ref="C2" r:id="rId13" xr:uid="{474DDF44-173E-49F7-BF59-B58BB733B18D}"/>
+    <hyperlink ref="V8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="W8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B12" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F17" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F21" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F25" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F30" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F5" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Braun Us updated code with new scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/BraunHC/BraunHCTestData.xlsx
+++ b/src/test/resources/TestData/BraunHC/BraunHCTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stage1\HoT-digital\src\test\resources\TestData\BraunHC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3AF648-6555-4F43-B9C8-696101DEFB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE83E13-9CCE-4B94-9F4F-14ECEC8D5CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="157">
   <si>
     <t>DataSet</t>
   </si>
@@ -232,9 +232,6 @@
   </si>
   <si>
     <t>HeaderLinks</t>
-  </si>
-  <si>
-    <t>Collections,Dryers,Straighteners,Curling Irons,Hair Brushes &amp; Elastics,Specialty</t>
   </si>
   <si>
     <t>HeaderMobileLinks</t>
@@ -452,6 +449,63 @@
   </si>
   <si>
     <t>Guam</t>
+  </si>
+  <si>
+    <t>Sortby</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>productprice</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Qunty</t>
+  </si>
+  <si>
+    <t>Education,Choosing the right thermometer,Ten tips about temperature checks,What is a fever?,Wellness Resources,5 most common home emergencies &amp; how to prepare</t>
+  </si>
+  <si>
+    <t>headermenu</t>
+  </si>
+  <si>
+    <t>megamenus</t>
+  </si>
+  <si>
+    <t>Thermometers,Nasal Aspirator,Blood Pressure Monitors,Pulse Oximeter,Parts &amp; Accessories</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Thermometers - Shop,Braun Nasal Aspirator - BNA100,Braun ExactFit 3 Upper Arm Blood Pressure Monitor,Braun Pulse Oximeter,Braun ThermoScan Lens Filters - LF40</t>
+  </si>
+  <si>
+    <t>Learnmenu</t>
+  </si>
+  <si>
+    <t>blog,choosing-the-right-thermometer,ten-tips-about-temperature-checks,what-is-a-fever,blog,5-most-common-home-emergencies-and-how-to-prepare</t>
+  </si>
+  <si>
+    <t>supportmenu</t>
+  </si>
+  <si>
+    <t>FAQs,Warranty Registration,Order Status</t>
+  </si>
+  <si>
+    <t>FAQ Support - Braun,Warranty,Orders and Returns</t>
+  </si>
+  <si>
+    <t>footersupport</t>
+  </si>
+  <si>
+    <t>Product Support,FAQs,Warranty Registration,Contact Us</t>
   </si>
 </sst>
 </file>
@@ -461,7 +515,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,6 +560,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -565,7 +627,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -594,6 +656,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -909,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN30"/>
+  <dimension ref="A1:AR36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="AE25" workbookViewId="0">
+      <selection activeCell="AF36" sqref="AF36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,17 +999,21 @@
     <col min="23" max="23" width="15.140625" customWidth="1"/>
     <col min="24" max="24" width="14.140625" customWidth="1"/>
     <col min="25" max="25" width="17.42578125" customWidth="1"/>
-    <col min="31" max="31" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22" customWidth="1"/>
-    <col min="33" max="33" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.42578125" customWidth="1"/>
-    <col min="35" max="35" width="29.42578125" customWidth="1"/>
-    <col min="36" max="36" width="16.5703125" customWidth="1"/>
-    <col min="37" max="37" width="22.5703125" customWidth="1"/>
-    <col min="40" max="40" width="28.140625" customWidth="1"/>
+    <col min="30" max="30" width="25.28515625" customWidth="1"/>
+    <col min="31" max="31" width="91.7109375" style="12" customWidth="1"/>
+    <col min="32" max="32" width="96.5703125" style="12" customWidth="1"/>
+    <col min="33" max="33" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22" customWidth="1"/>
+    <col min="35" max="35" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.42578125" customWidth="1"/>
+    <col min="37" max="37" width="29.42578125" customWidth="1"/>
+    <col min="38" max="38" width="16.5703125" customWidth="1"/>
+    <col min="39" max="39" width="22.5703125" customWidth="1"/>
+    <col min="42" max="42" width="28.140625" customWidth="1"/>
+    <col min="43" max="43" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -987,7 +1054,7 @@
         <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>12</v>
@@ -1038,109 +1105,121 @@
         <v>27</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AN1" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:40" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="AP1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>52</v>
@@ -1152,20 +1231,20 @@
         <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>53</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M5" s="3">
         <v>9898989899</v>
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1186,7 +1265,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1207,7 +1286,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1227,18 +1306,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G9" t="s">
         <v>32</v>
@@ -1250,7 +1329,7 @@
         <v>47</v>
       </c>
       <c r="J9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K9" t="s">
         <v>48</v>
@@ -1284,18 +1363,18 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G10" t="s">
         <v>52</v>
@@ -1307,10 +1386,10 @@
         <v>34</v>
       </c>
       <c r="J10" t="s">
+        <v>103</v>
+      </c>
+      <c r="K10" t="s">
         <v>104</v>
-      </c>
-      <c r="K10" t="s">
-        <v>105</v>
       </c>
       <c r="L10" s="6">
         <v>98569</v>
@@ -1319,10 +1398,10 @@
         <v>9898989899</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1330,7 +1409,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1341,41 +1420,41 @@
         <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J13">
         <f>+K11</f>
         <v>0</v>
       </c>
       <c r="T13" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>59</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1383,15 +1462,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC17" t="s">
         <v>63</v>
@@ -1400,45 +1479,45 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:44" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
-      <c r="AE18" t="s">
+      <c r="AG18" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="AG19" t="s">
         <v>67</v>
       </c>
-      <c r="AE19" t="s">
+    </row>
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="T20" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="AH20" t="s">
         <v>84</v>
       </c>
-      <c r="T20" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G21" t="s">
         <v>32</v>
@@ -1450,7 +1529,7 @@
         <v>47</v>
       </c>
       <c r="J21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K21" t="s">
         <v>53</v>
@@ -1462,19 +1541,19 @@
         <v>9898989899</v>
       </c>
       <c r="N21" s="3"/>
-      <c r="AG21">
+      <c r="AI21">
         <v>8444</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="O22" t="s">
         <v>73</v>
       </c>
-      <c r="O22" t="s">
-        <v>74</v>
-      </c>
       <c r="P22" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q22">
         <v>2030</v>
@@ -1486,15 +1565,15 @@
         <v>731</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>80</v>
+      </c>
+      <c r="O23" t="s">
         <v>81</v>
       </c>
-      <c r="O23" t="s">
-        <v>82</v>
-      </c>
       <c r="P23" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q23">
         <v>2030</v>
@@ -1506,15 +1585,15 @@
         <v>731</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="O24" t="s">
         <v>76</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="P24" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="Q24" s="12">
         <v>2030</v>
@@ -1525,34 +1604,34 @@
       <c r="S24">
         <v>9876</v>
       </c>
-      <c r="AH24">
+      <c r="AJ24">
         <v>25376</v>
       </c>
-      <c r="AI24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AK24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" t="s">
         <v>90</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G25" t="s">
-        <v>89</v>
-      </c>
-      <c r="I25" t="s">
-        <v>90</v>
-      </c>
-      <c r="J25" t="s">
-        <v>91</v>
       </c>
       <c r="K25" t="s">
         <v>35</v>
@@ -1564,48 +1643,48 @@
         <v>8897006543</v>
       </c>
       <c r="T25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Y25" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH25">
+        <v>126</v>
+      </c>
+      <c r="AJ25">
         <v>9876543210</v>
       </c>
-      <c r="AI25" t="s">
+      <c r="AK25" t="s">
+        <v>131</v>
+      </c>
+      <c r="AL25">
+        <v>56789</v>
+      </c>
+    </row>
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" t="s">
         <v>132</v>
       </c>
-      <c r="AJ25">
-        <v>56789</v>
-      </c>
-    </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>133</v>
       </c>
-      <c r="E26" t="s">
-        <v>134</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G26" t="s">
+        <v>91</v>
+      </c>
+      <c r="H26" t="s">
         <v>92</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>93</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>94</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>95</v>
-      </c>
-      <c r="K26" t="s">
-        <v>96</v>
       </c>
       <c r="L26">
         <v>98987</v>
@@ -1614,47 +1693,50 @@
         <v>9898908878</v>
       </c>
       <c r="T26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Y26" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK26">
+        <v>126</v>
+      </c>
+      <c r="AM26">
         <v>3400000747</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM27">
+        <v>107</v>
+      </c>
+      <c r="AP27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AR27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" t="s">
         <v>110</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>111</v>
-      </c>
-      <c r="E28" t="s">
-        <v>112</v>
       </c>
       <c r="G28" t="s">
         <v>32</v>
       </c>
       <c r="H28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I28" t="s">
         <v>47</v>
       </c>
       <c r="J28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L28">
         <v>71823</v>
@@ -1663,30 +1745,30 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" t="s">
         <v>113</v>
       </c>
-      <c r="D29" t="s">
-        <v>111</v>
-      </c>
-      <c r="E29" t="s">
-        <v>114</v>
-      </c>
       <c r="G29" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L29" s="12">
         <v>60026</v>
@@ -1695,39 +1777,99 @@
         <v>8897006543</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G30" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>120</v>
-      </c>
       <c r="H30" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>47</v>
       </c>
       <c r="J30" t="s">
+        <v>120</v>
+      </c>
+      <c r="K30" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="K30" s="14" t="s">
-        <v>122</v>
-      </c>
       <c r="L30" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M30" s="12">
         <v>8897006543</v>
+      </c>
+    </row>
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>138</v>
+      </c>
+      <c r="AQ31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE32" s="18"/>
+      <c r="AF32" s="18"/>
+      <c r="AQ32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE33" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AF33" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>150</v>
+      </c>
+      <c r="AE34" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF34" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="AE35" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF35" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE36" s="12" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committed BVT and smoke test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/BraunHC/BraunHCTestData.xlsx
+++ b/src/test/resources/TestData/BraunHC/BraunHCTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stage1\HoT-digital\src\test\resources\TestData\BraunHC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\HoT-digital\src\test\resources\TestData\BraunHC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE83E13-9CCE-4B94-9F4F-14ECEC8D5CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52663FC9-2569-479F-B117-9F4486A6F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="164">
   <si>
     <t>DataSet</t>
   </si>
@@ -232,9 +232,6 @@
   </si>
   <si>
     <t>HeaderLinks</t>
-  </si>
-  <si>
-    <t>HeaderMobileLinks</t>
   </si>
   <si>
     <t>Dryers,Straighteners,Curling Irons,Hair Brushes &amp; Elastics,Specialty</t>
@@ -496,16 +493,40 @@
     <t>supportmenu</t>
   </si>
   <si>
-    <t>FAQs,Warranty Registration,Order Status</t>
-  </si>
-  <si>
-    <t>FAQ Support - Braun,Warranty,Orders and Returns</t>
-  </si>
-  <si>
     <t>footersupport</t>
   </si>
   <si>
     <t>Product Support,FAQs,Warranty Registration,Contact Us</t>
+  </si>
+  <si>
+    <t>ShippingAddress</t>
+  </si>
+  <si>
+    <t>845 N Colony Rd</t>
+  </si>
+  <si>
+    <t>06493</t>
+  </si>
+  <si>
+    <t>Therom</t>
+  </si>
+  <si>
+    <t>RelatedproductNames</t>
+  </si>
+  <si>
+    <t>relatedprodcuts</t>
+  </si>
+  <si>
+    <t>Relatedproduct</t>
+  </si>
+  <si>
+    <t>Warranty Registration,Order Status</t>
+  </si>
+  <si>
+    <t>Warranty,Orders and Returns</t>
+  </si>
+  <si>
+    <t>BSTGUS3400007089</t>
   </si>
 </sst>
 </file>
@@ -972,10 +993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR36"/>
+  <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE25" workbookViewId="0">
-      <selection activeCell="AF36" sqref="AF36"/>
+    <sheetView tabSelected="1" topLeftCell="AJ10" workbookViewId="0">
+      <selection activeCell="AO18" sqref="AO18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,32 +1009,36 @@
     <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="23" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
     <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.140625" customWidth="1"/>
-    <col min="24" max="24" width="14.140625" customWidth="1"/>
-    <col min="25" max="25" width="17.42578125" customWidth="1"/>
-    <col min="30" max="30" width="25.28515625" customWidth="1"/>
-    <col min="31" max="31" width="91.7109375" style="12" customWidth="1"/>
-    <col min="32" max="32" width="96.5703125" style="12" customWidth="1"/>
-    <col min="33" max="33" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22" customWidth="1"/>
-    <col min="35" max="35" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.42578125" customWidth="1"/>
-    <col min="37" max="37" width="29.42578125" customWidth="1"/>
-    <col min="38" max="38" width="16.5703125" customWidth="1"/>
-    <col min="39" max="39" width="22.5703125" customWidth="1"/>
-    <col min="42" max="42" width="28.140625" customWidth="1"/>
-    <col min="43" max="43" width="22.7109375" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="12"/>
+    <col min="21" max="21" width="22.42578125" style="12" customWidth="1"/>
+    <col min="22" max="22" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" customWidth="1"/>
+    <col min="26" max="26" width="14.140625" customWidth="1"/>
+    <col min="27" max="27" width="17.42578125" customWidth="1"/>
+    <col min="32" max="32" width="25.28515625" customWidth="1"/>
+    <col min="33" max="33" width="91.7109375" style="12" customWidth="1"/>
+    <col min="34" max="34" width="96.5703125" style="12" customWidth="1"/>
+    <col min="35" max="35" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="22" customWidth="1"/>
+    <col min="37" max="37" width="17.42578125" customWidth="1"/>
+    <col min="38" max="38" width="30.42578125" customWidth="1"/>
+    <col min="39" max="39" width="30.140625" customWidth="1"/>
+    <col min="40" max="40" width="25" customWidth="1"/>
+    <col min="41" max="41" width="22.5703125" customWidth="1"/>
+    <col min="42" max="42" width="20.140625" customWidth="1"/>
+    <col min="44" max="44" width="28.140625" customWidth="1"/>
+    <col min="45" max="45" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1079,7 @@
         <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>12</v>
@@ -1072,154 +1097,160 @@
         <v>16</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="AG1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AK1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AN1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AP1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="AR1" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>52</v>
@@ -1231,20 +1262,20 @@
         <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>53</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M5" s="3">
         <v>9898989899</v>
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1264,8 +1295,10 @@
       <c r="S6" s="3">
         <v>737</v>
       </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1285,39 +1318,41 @@
       <c r="S7" s="3">
         <v>737</v>
       </c>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="2"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
-      <c r="T8" t="s">
+      <c r="V8" t="s">
         <v>43</v>
       </c>
-      <c r="U8" t="s">
+      <c r="W8" t="s">
         <v>44</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="Y8" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G9" t="s">
         <v>32</v>
@@ -1329,7 +1364,7 @@
         <v>47</v>
       </c>
       <c r="J9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K9" t="s">
         <v>48</v>
@@ -1341,40 +1376,40 @@
         <v>9898989899</v>
       </c>
       <c r="N9" s="3"/>
-      <c r="T9" t="s">
+      <c r="V9" t="s">
         <v>43</v>
       </c>
-      <c r="U9" t="s">
+      <c r="W9" t="s">
         <v>49</v>
       </c>
-      <c r="X9">
+      <c r="Z9">
         <v>12341</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="AA9" t="s">
         <v>50</v>
       </c>
-      <c r="Z9">
+      <c r="AB9">
         <v>5</v>
       </c>
-      <c r="AA9">
+      <c r="AC9">
         <v>6</v>
       </c>
-      <c r="AB9">
+      <c r="AD9">
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G10" t="s">
         <v>52</v>
@@ -1386,10 +1421,10 @@
         <v>34</v>
       </c>
       <c r="J10" t="s">
+        <v>102</v>
+      </c>
+      <c r="K10" t="s">
         <v>103</v>
-      </c>
-      <c r="K10" t="s">
-        <v>104</v>
       </c>
       <c r="L10" s="6">
         <v>98569</v>
@@ -1398,18 +1433,18 @@
         <v>9898989899</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="T11" t="s">
+      <c r="V11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1420,104 +1455,107 @@
         <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J13">
         <f>+K11</f>
         <v>0</v>
       </c>
-      <c r="T13" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="U13" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>59</v>
       </c>
-      <c r="T15" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="V15" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
-      <c r="T16" s="6" t="s">
+      <c r="V16" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE17" t="s">
         <v>63</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AF17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:44" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
-      <c r="AG18" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AI18" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI19" t="s">
         <v>66</v>
       </c>
-      <c r="AG19" t="s">
+    </row>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="V20" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="AJ20" t="s">
         <v>83</v>
       </c>
-      <c r="T20" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G21" t="s">
         <v>32</v>
@@ -1529,7 +1567,7 @@
         <v>47</v>
       </c>
       <c r="J21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K21" t="s">
         <v>53</v>
@@ -1541,19 +1579,19 @@
         <v>9898989899</v>
       </c>
       <c r="N21" s="3"/>
-      <c r="AI21">
+      <c r="AK21">
         <v>8444</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="O22" t="s">
         <v>72</v>
       </c>
-      <c r="O22" t="s">
-        <v>73</v>
-      </c>
       <c r="P22" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q22">
         <v>2030</v>
@@ -1565,15 +1603,15 @@
         <v>731</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="O23" t="s">
         <v>80</v>
       </c>
-      <c r="O23" t="s">
-        <v>81</v>
-      </c>
       <c r="P23" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q23">
         <v>2030</v>
@@ -1585,15 +1623,15 @@
         <v>731</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="O24" t="s">
         <v>75</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="P24" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="Q24" s="12">
         <v>2030</v>
@@ -1604,34 +1642,34 @@
       <c r="S24">
         <v>9876</v>
       </c>
-      <c r="AJ24">
+      <c r="AL24">
         <v>25376</v>
       </c>
-      <c r="AK24" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AM24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G25" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" t="s">
+        <v>88</v>
+      </c>
+      <c r="J25" t="s">
         <v>89</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G25" t="s">
-        <v>88</v>
-      </c>
-      <c r="I25" t="s">
-        <v>89</v>
-      </c>
-      <c r="J25" t="s">
-        <v>90</v>
       </c>
       <c r="K25" t="s">
         <v>35</v>
@@ -1642,49 +1680,49 @@
       <c r="M25">
         <v>8897006543</v>
       </c>
-      <c r="T25" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y25" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="AJ25">
+      <c r="V25" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA25" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="AL25">
         <v>9876543210</v>
       </c>
-      <c r="AK25" t="s">
+      <c r="AM25" t="s">
+        <v>130</v>
+      </c>
+      <c r="AN25">
+        <v>3400089</v>
+      </c>
+    </row>
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
         <v>131</v>
       </c>
-      <c r="AL25">
-        <v>56789</v>
-      </c>
-    </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>132</v>
       </c>
-      <c r="E26" t="s">
-        <v>133</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G26" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" t="s">
         <v>91</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>92</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>93</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>94</v>
-      </c>
-      <c r="K26" t="s">
-        <v>95</v>
       </c>
       <c r="L26">
         <v>98987</v>
@@ -1692,51 +1730,51 @@
       <c r="M26">
         <v>9898908878</v>
       </c>
-      <c r="T26" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM26">
-        <v>3400000747</v>
-      </c>
-    </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="V26" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>125</v>
+      </c>
+      <c r="AP26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>107</v>
-      </c>
-      <c r="AP27">
+        <v>106</v>
+      </c>
+      <c r="AR27">
         <v>2</v>
       </c>
-      <c r="AR27">
+      <c r="AT27">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" t="s">
         <v>109</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>110</v>
-      </c>
-      <c r="E28" t="s">
-        <v>111</v>
       </c>
       <c r="G28" t="s">
         <v>32</v>
       </c>
       <c r="H28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I28" t="s">
         <v>47</v>
       </c>
       <c r="J28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L28">
         <v>71823</v>
@@ -1745,30 +1783,30 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" t="s">
         <v>112</v>
       </c>
-      <c r="D29" t="s">
-        <v>110</v>
-      </c>
-      <c r="E29" t="s">
-        <v>113</v>
-      </c>
       <c r="G29" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L29" s="12">
         <v>60026</v>
@@ -1777,106 +1815,151 @@
         <v>8897006543</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G30" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>119</v>
-      </c>
       <c r="H30" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>47</v>
       </c>
       <c r="J30" t="s">
+        <v>119</v>
+      </c>
+      <c r="K30" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="K30" s="14" t="s">
-        <v>121</v>
-      </c>
       <c r="L30" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M30" s="12">
         <v>8897006543</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>138</v>
-      </c>
-      <c r="AQ31" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="AG32" s="18"/>
+      <c r="AH32" s="18"/>
+      <c r="AS32" t="s">
         <v>141</v>
       </c>
-      <c r="AE32" s="18"/>
-      <c r="AF32" s="18"/>
-      <c r="AQ32" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>145</v>
-      </c>
-      <c r="AE33" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="AF33" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG33" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="AH33" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="34" spans="1:32" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="AG34" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH34" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="AE34" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="AF34" s="7" t="s">
+    </row>
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="F35" s="12"/>
+      <c r="AG35" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="AH35" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>152</v>
       </c>
-      <c r="F35" s="12"/>
-      <c r="AE35" s="12" t="s">
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="3"/>
+      <c r="AG36" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="AF35" s="12" t="s">
+    </row>
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="D37" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G37" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="AE36" s="12" t="s">
+      <c r="H37" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L37" s="15" t="s">
         <v>156</v>
+      </c>
+      <c r="M37" s="3">
+        <v>9898989899</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="V8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="W8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="X8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="Y8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="F9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B12" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="F10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
@@ -1887,8 +1970,9 @@
     <hyperlink ref="F30" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="F5" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="F4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F37" r:id="rId13" xr:uid="{02075A1C-ECAF-4BBA-9BFC-D744BC9C79A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BraunUS and Febreze Upadate code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/BraunHC/BraunHCTestData.xlsx
+++ b/src/test/resources/TestData/BraunHC/BraunHCTestData.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\HoT-digital\src\test\resources\TestData\BraunHC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkJEE!\braunUS\new code 04-01-21\HoT-digital\src\test\resources\TestData\BraunHC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52663FC9-2569-479F-B117-9F4486A6F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ACADA8-226F-4EAF-A419-EEE72512968F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="165">
   <si>
     <t>DataSet</t>
   </si>
@@ -527,6 +525,9 @@
   </si>
   <si>
     <t>BSTGUS3400007089</t>
+  </si>
+  <si>
+    <t>BraunUS</t>
   </si>
 </sst>
 </file>
@@ -995,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ10" workbookViewId="0">
-      <selection activeCell="AO18" sqref="AO18"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,7 +1550,7 @@
         <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>116</v>
+        <v>164</v>
       </c>
       <c r="E21" t="s">
         <v>88</v>

</xml_diff>